<commit_message>
add test for Campbell2003 and Toro2002
</commit_message>
<xml_diff>
--- a/test_data/Toro02_MEDIAN_NotAdjusted.xlsx
+++ b/test_data/Toro02_MEDIAN_NotAdjusted.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="20" windowWidth="33180" windowHeight="23100" tabRatio="500"/>
+    <workbookView xWindow="2280" yWindow="20" windowWidth="33180" windowHeight="23100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Toro02_MEDIAN_NotAdjusted.OUT" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PGV</t>
+    <t>h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>PGV</t>
   </si>
 </sst>
 </file>
@@ -45,7 +44,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -77,9 +76,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,18 +409,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="4" max="15" width="10.7109375" style="1"/>
+    <col min="4" max="13" width="10.7109375" style="1"/>
+    <col min="14" max="14" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1">
         <v>2.86E-2</v>
@@ -446,28 +447,25 @@
         <v>0.4</v>
       </c>
       <c r="I1" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K1" s="1">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="1">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1">
+      <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>5</v>
       </c>
@@ -493,31 +491,27 @@
         <v>0.129</v>
       </c>
       <c r="I2" s="1">
-        <v>5.0853369994483498E-2</v>
+        <v>3.3300000000000003E-2</v>
       </c>
       <c r="J2" s="1">
-        <v>3.3300000000000003E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="K2" s="1">
-        <v>8.0000000000000002E-3</v>
+        <f>J2*0.559</f>
+        <v>4.4720000000000003E-3</v>
       </c>
       <c r="L2" s="1">
-        <f>K2*0.559</f>
-        <v>4.4720000000000003E-3</v>
+        <f>J2*0.612</f>
+        <v>4.8960000000000002E-3</v>
       </c>
       <c r="M2" s="1">
-        <f>K2*0.612</f>
-        <v>4.8960000000000002E-3</v>
-      </c>
-      <c r="N2" s="1">
         <v>0.22020000000000001</v>
       </c>
-      <c r="O2" s="1">
-        <f>I2*981/20</f>
+      <c r="N2" s="2">
         <v>2.4943577982294154</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>5</v>
       </c>
@@ -543,31 +537,27 @@
         <v>8.9200000000000002E-2</v>
       </c>
       <c r="I3" s="1">
-        <v>3.51739361432305E-2</v>
+        <v>2.3099999999999999E-2</v>
       </c>
       <c r="J3" s="1">
-        <v>2.3099999999999999E-2</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="K3" s="1">
-        <v>5.4999999999999997E-3</v>
+        <f t="shared" ref="K3:K66" si="0">J3*0.559</f>
+        <v>3.0745E-3</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L66" si="0">K3*0.559</f>
-        <v>3.0745E-3</v>
+        <f t="shared" ref="L3:L66" si="1">J3*0.612</f>
+        <v>3.3659999999999996E-3</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M66" si="1">K3*0.612</f>
-        <v>3.3659999999999996E-3</v>
-      </c>
-      <c r="N3" s="1">
         <v>0.15049999999999999</v>
       </c>
-      <c r="O3" s="1">
-        <f t="shared" ref="O3:O66" si="2">I3*981/20</f>
+      <c r="N3" s="2">
         <v>1.7252815678254561</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>5</v>
       </c>
@@ -593,31 +583,27 @@
         <v>5.0799999999999998E-2</v>
       </c>
       <c r="I4" s="1">
-        <v>2.0103232849344399E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="J4" s="1">
-        <v>1.34E-2</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="K4" s="1">
-        <v>3.2000000000000002E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.7888000000000003E-3</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7888000000000003E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.9583999999999999E-3</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="1"/>
-        <v>1.9583999999999999E-3</v>
-      </c>
-      <c r="N4" s="1">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="O4" s="1">
-        <f t="shared" si="2"/>
+      <c r="N4" s="2">
         <v>0.98606357126034272</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>5</v>
       </c>
@@ -643,31 +629,27 @@
         <v>3.4599999999999999E-2</v>
       </c>
       <c r="I5" s="1">
-        <v>1.37245846224852E-2</v>
+        <v>9.2999999999999992E-3</v>
       </c>
       <c r="J5" s="1">
-        <v>9.2999999999999992E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="K5" s="1">
-        <v>2.2000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.2298000000000003E-3</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2298000000000003E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.3464E-3</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="1"/>
-        <v>1.3464E-3</v>
-      </c>
-      <c r="N5" s="1">
         <v>4.7800000000000002E-2</v>
       </c>
-      <c r="O5" s="1">
-        <f t="shared" si="2"/>
+      <c r="N5" s="2">
         <v>0.67319087573289904</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>5</v>
       </c>
@@ -693,31 +675,27 @@
         <v>2.0400000000000001E-2</v>
       </c>
       <c r="I6" s="1">
-        <v>8.1457326516057305E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="J6" s="1">
-        <v>5.7000000000000002E-3</v>
+        <v>1.4E-3</v>
       </c>
       <c r="K6" s="1">
-        <v>1.4E-3</v>
+        <f t="shared" si="0"/>
+        <v>7.8260000000000005E-4</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="0"/>
-        <v>7.8260000000000005E-4</v>
+        <f t="shared" si="1"/>
+        <v>8.5680000000000001E-4</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="1"/>
-        <v>8.5680000000000001E-4</v>
-      </c>
-      <c r="N6" s="1">
         <v>2.47E-2</v>
       </c>
-      <c r="O6" s="1">
-        <f t="shared" si="2"/>
+      <c r="N6" s="2">
         <v>0.39954818656126107</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>5</v>
       </c>
@@ -743,31 +721,27 @@
         <v>1.29E-2</v>
       </c>
       <c r="I7" s="1">
-        <v>5.1997500026796104E-3</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="J7" s="1">
-        <v>3.7000000000000002E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="K7" s="1">
-        <v>8.9999999999999998E-4</v>
+        <f t="shared" si="0"/>
+        <v>5.0310000000000003E-4</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="0"/>
-        <v>5.0310000000000003E-4</v>
+        <f t="shared" si="1"/>
+        <v>5.5079999999999994E-4</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="1"/>
-        <v>5.5079999999999994E-4</v>
-      </c>
-      <c r="N7" s="1">
         <v>1.41E-2</v>
       </c>
-      <c r="O7" s="1">
-        <f t="shared" si="2"/>
+      <c r="N7" s="2">
         <v>0.2550477376314349</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>5</v>
       </c>
@@ -793,31 +767,27 @@
         <v>9.1000000000000004E-3</v>
       </c>
       <c r="I8" s="1">
-        <v>3.69364933089379E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="J8" s="1">
-        <v>2.7000000000000001E-3</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="K8" s="1">
-        <v>6.9999999999999999E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.9130000000000002E-4</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="0"/>
-        <v>3.9130000000000002E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.284E-4</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="1"/>
-        <v>4.284E-4</v>
-      </c>
-      <c r="N8" s="1">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="O8" s="1">
-        <f t="shared" si="2"/>
+      <c r="N8" s="2">
         <v>0.18117349968034041</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>5</v>
       </c>
@@ -843,31 +813,27 @@
         <v>4.4999999999999997E-3</v>
       </c>
       <c r="I9" s="1">
-        <v>1.8490662820124799E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="J9" s="1">
-        <v>1.5E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="K9" s="1">
-        <v>4.0000000000000002E-4</v>
+        <f t="shared" si="0"/>
+        <v>2.2360000000000004E-4</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2360000000000004E-4</v>
+        <f t="shared" si="1"/>
+        <v>2.4479999999999999E-4</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="1"/>
-        <v>2.4479999999999999E-4</v>
-      </c>
-      <c r="N9" s="1">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="O9" s="1">
-        <f t="shared" si="2"/>
+      <c r="N9" s="2">
         <v>9.0696701132712138E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>5</v>
       </c>
@@ -893,31 +859,27 @@
         <v>1E-3</v>
       </c>
       <c r="I10" s="1">
-        <v>4.3766178297936201E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="J10" s="1">
-        <v>5.0000000000000001E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="K10" s="1">
-        <v>2.0000000000000001E-4</v>
+        <f t="shared" si="0"/>
+        <v>1.1180000000000002E-4</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1180000000000002E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.2239999999999999E-4</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2239999999999999E-4</v>
-      </c>
-      <c r="N10" s="1">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="O10" s="1">
-        <f t="shared" si="2"/>
+      <c r="N10" s="2">
         <v>2.1467310455137705E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>5</v>
       </c>
@@ -943,31 +905,27 @@
         <v>1E-4</v>
       </c>
       <c r="I11" s="1">
-        <v>6.2582651159156995E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <v>1E-4</v>
       </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="O11" s="1">
-        <f t="shared" si="2"/>
+      <c r="N11" s="2">
         <v>3.0696790393566508E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>5.5</v>
       </c>
@@ -993,31 +951,27 @@
         <v>0.21920000000000001</v>
       </c>
       <c r="I12" s="1">
-        <v>8.3474161777531003E-2</v>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="J12" s="1">
-        <v>7.3700000000000002E-2</v>
+        <v>2.3900000000000001E-2</v>
       </c>
       <c r="K12" s="1">
-        <v>2.3900000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.3360100000000001E-2</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="0"/>
-        <v>1.3360100000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4626800000000001E-2</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="1"/>
-        <v>1.4626800000000001E-2</v>
-      </c>
-      <c r="N12" s="1">
         <v>0.29549999999999998</v>
       </c>
-      <c r="O12" s="1">
-        <f t="shared" si="2"/>
+      <c r="N12" s="2">
         <v>4.0944076351878955</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>5.5</v>
       </c>
@@ -1043,31 +997,27 @@
         <v>0.157</v>
       </c>
       <c r="I13" s="1">
-        <v>5.9818945554624199E-2</v>
+        <v>5.28E-2</v>
       </c>
       <c r="J13" s="1">
-        <v>5.28E-2</v>
+        <v>1.72E-2</v>
       </c>
       <c r="K13" s="1">
-        <v>1.72E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.6148000000000015E-3</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="0"/>
-        <v>9.6148000000000015E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.05264E-2</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="1"/>
-        <v>1.05264E-2</v>
-      </c>
-      <c r="N13" s="1">
         <v>0.2117</v>
       </c>
-      <c r="O13" s="1">
-        <f t="shared" si="2"/>
+      <c r="N13" s="2">
         <v>2.9341192794543169</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>5.5</v>
       </c>
@@ -1093,31 +1043,27 @@
         <v>9.1499999999999998E-2</v>
       </c>
       <c r="I14" s="1">
-        <v>3.4960116969387202E-2</v>
+        <v>3.1300000000000001E-2</v>
       </c>
       <c r="J14" s="1">
-        <v>3.1300000000000001E-2</v>
+        <v>1.01E-2</v>
       </c>
       <c r="K14" s="1">
-        <v>1.01E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.6459000000000006E-3</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="0"/>
-        <v>5.6459000000000006E-3</v>
+        <f t="shared" si="1"/>
+        <v>6.1811999999999995E-3</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="1"/>
-        <v>6.1811999999999995E-3</v>
-      </c>
-      <c r="N14" s="1">
         <v>0.11310000000000001</v>
       </c>
-      <c r="O14" s="1">
-        <f t="shared" si="2"/>
+      <c r="N14" s="2">
         <v>1.7147937373484421</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>5.5</v>
       </c>
@@ -1143,31 +1089,27 @@
         <v>6.2700000000000006E-2</v>
       </c>
       <c r="I15" s="1">
-        <v>2.4005754430358701E-2</v>
+        <v>2.18E-2</v>
       </c>
       <c r="J15" s="1">
-        <v>2.18E-2</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="K15" s="1">
-        <v>7.1000000000000004E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.9689000000000009E-3</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="0"/>
-        <v>3.9689000000000009E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.3452000000000005E-3</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="1"/>
-        <v>4.3452000000000005E-3</v>
-      </c>
-      <c r="N15" s="1">
         <v>7.0800000000000002E-2</v>
       </c>
-      <c r="O15" s="1">
-        <f t="shared" si="2"/>
+      <c r="N15" s="2">
         <v>1.1774822548090942</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>5.5</v>
       </c>
@@ -1193,31 +1135,27 @@
         <v>3.7100000000000001E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>1.42948285961034E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="J16" s="1">
-        <v>1.34E-2</v>
+        <v>4.3E-3</v>
       </c>
       <c r="K16" s="1">
-        <v>4.3E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.4037000000000004E-3</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="0"/>
-        <v>2.4037000000000004E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.6316E-3</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="1"/>
-        <v>2.6316E-3</v>
-      </c>
-      <c r="N16" s="1">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="O16" s="1">
-        <f t="shared" si="2"/>
+      <c r="N16" s="2">
         <v>0.70116134263887175</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>5.5</v>
       </c>
@@ -1243,31 +1181,27 @@
         <v>2.3599999999999999E-2</v>
       </c>
       <c r="I17" s="1">
-        <v>9.1351120538628004E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="J17" s="1">
-        <v>8.8000000000000005E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="K17" s="1">
-        <v>2.8999999999999998E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.6211000000000001E-3</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6211000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.7747999999999998E-3</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7747999999999998E-3</v>
-      </c>
-      <c r="N17" s="1">
         <v>2.1100000000000001E-2</v>
       </c>
-      <c r="O17" s="1">
-        <f t="shared" si="2"/>
+      <c r="N17" s="2">
         <v>0.44807724624197032</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>5.5</v>
       </c>
@@ -1293,31 +1227,27 @@
         <v>1.67E-2</v>
       </c>
       <c r="I18" s="1">
-        <v>6.4930225320027199E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="J18" s="1">
-        <v>6.4000000000000003E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="K18" s="1">
-        <v>2.0999999999999999E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.1739000000000001E-3</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1739000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.2851999999999998E-3</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2851999999999998E-3</v>
-      </c>
-      <c r="N18" s="1">
         <v>1.4E-2</v>
       </c>
-      <c r="O18" s="1">
-        <f t="shared" si="2"/>
+      <c r="N18" s="2">
         <v>0.3184827551947334</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>5.5</v>
       </c>
@@ -1343,31 +1273,27 @@
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="I19" s="1">
-        <v>3.2513757124613E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="J19" s="1">
-        <v>3.5999999999999999E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="K19" s="1">
-        <v>1.2999999999999999E-3</v>
+        <f t="shared" si="0"/>
+        <v>7.2670000000000005E-4</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="0"/>
-        <v>7.2670000000000005E-4</v>
+        <f t="shared" si="1"/>
+        <v>7.9559999999999993E-4</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="1"/>
-        <v>7.9559999999999993E-4</v>
-      </c>
-      <c r="N19" s="1">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="O19" s="1">
-        <f t="shared" si="2"/>
+      <c r="N19" s="2">
         <v>0.15947997869622677</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>5.5</v>
       </c>
@@ -1393,31 +1319,27 @@
         <v>1.8E-3</v>
       </c>
       <c r="I20" s="1">
-        <v>7.6966003032766901E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="J20" s="1">
-        <v>1.1999999999999999E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K20" s="1">
-        <v>5.0000000000000001E-4</v>
+        <f t="shared" si="0"/>
+        <v>2.7950000000000002E-4</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="0"/>
-        <v>2.7950000000000002E-4</v>
+        <f t="shared" si="1"/>
+        <v>3.0600000000000001E-4</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="1"/>
-        <v>3.0600000000000001E-4</v>
-      </c>
-      <c r="N20" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="O20" s="1">
-        <f t="shared" si="2"/>
+      <c r="N20" s="2">
         <v>3.7751824487572166E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>5.5</v>
       </c>
@@ -1443,31 +1365,27 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="I21" s="1">
-        <v>1.10058780824761E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="J21" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="K21" s="1">
-        <v>2.0000000000000001E-4</v>
+        <f t="shared" si="0"/>
+        <v>1.1180000000000002E-4</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1180000000000002E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.2239999999999999E-4</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2239999999999999E-4</v>
-      </c>
-      <c r="N21" s="1">
         <v>1E-4</v>
       </c>
-      <c r="O21" s="1">
-        <f t="shared" si="2"/>
+      <c r="N21" s="2">
         <v>5.3983831994545272E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:14">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1493,31 +1411,27 @@
         <v>0.3523</v>
       </c>
       <c r="I22" s="1">
-        <v>0.13546110559402399</v>
+        <v>0.14680000000000001</v>
       </c>
       <c r="J22" s="1">
-        <v>0.14680000000000001</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="K22" s="1">
-        <v>6.0999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.4099000000000004E-2</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4099000000000004E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.7331999999999997E-2</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="1"/>
-        <v>3.7331999999999997E-2</v>
-      </c>
-      <c r="N22" s="1">
         <v>0.39429999999999998</v>
       </c>
-      <c r="O22" s="1">
-        <f t="shared" si="2"/>
+      <c r="N22" s="2">
         <v>6.6443672293868774</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:14">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1543,31 +1457,27 @@
         <v>0.2616</v>
       </c>
       <c r="I23" s="1">
-        <v>0.100581043987616</v>
+        <v>0.109</v>
       </c>
       <c r="J23" s="1">
-        <v>0.109</v>
+        <v>4.53E-2</v>
       </c>
       <c r="K23" s="1">
-        <v>4.53E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.5322700000000004E-2</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="0"/>
-        <v>2.5322700000000004E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.7723600000000001E-2</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="1"/>
-        <v>2.7723600000000001E-2</v>
-      </c>
-      <c r="N23" s="1">
         <v>0.29520000000000002</v>
       </c>
-      <c r="O23" s="1">
-        <f t="shared" si="2"/>
+      <c r="N23" s="2">
         <v>4.933500207592564</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:14">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1593,31 +1503,27 @@
         <v>0.15640000000000001</v>
       </c>
       <c r="I24" s="1">
-        <v>6.0291130031821002E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="J24" s="1">
-        <v>6.6100000000000006E-2</v>
+        <v>2.7400000000000001E-2</v>
       </c>
       <c r="K24" s="1">
-        <v>2.7400000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.5316600000000001E-2</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5316600000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.67688E-2</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="1"/>
-        <v>1.67688E-2</v>
-      </c>
-      <c r="N24" s="1">
         <v>0.1646</v>
       </c>
-      <c r="O24" s="1">
-        <f t="shared" si="2"/>
+      <c r="N24" s="2">
         <v>2.95727992806082</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:14">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1643,31 +1549,27 @@
         <v>0.10780000000000001</v>
       </c>
       <c r="I25" s="1">
-        <v>4.1689916606309101E-2</v>
+        <v>4.6399999999999997E-2</v>
       </c>
       <c r="J25" s="1">
-        <v>4.6399999999999997E-2</v>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="K25" s="1">
-        <v>1.9199999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0732800000000001E-2</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0732800000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.1750399999999999E-2</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1750399999999999E-2</v>
-      </c>
-      <c r="N25" s="1">
         <v>0.1045</v>
       </c>
-      <c r="O25" s="1">
-        <f t="shared" si="2"/>
+      <c r="N25" s="2">
         <v>2.0448904095394616</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:14">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1693,31 +1595,27 @@
         <v>6.4100000000000004E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>2.4926633687878199E-2</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="J26" s="1">
-        <v>2.8500000000000001E-2</v>
+        <v>1.18E-2</v>
       </c>
       <c r="K26" s="1">
-        <v>1.18E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.5962000000000008E-3</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="0"/>
-        <v>6.5962000000000008E-3</v>
+        <f t="shared" si="1"/>
+        <v>7.2215999999999999E-3</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="1"/>
-        <v>7.2215999999999999E-3</v>
-      </c>
-      <c r="N26" s="1">
         <v>5.4899999999999997E-2</v>
       </c>
-      <c r="O26" s="1">
-        <f t="shared" si="2"/>
+      <c r="N26" s="2">
         <v>1.2226513823904257</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:14">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1743,31 +1641,27 @@
         <v>4.0800000000000003E-2</v>
       </c>
       <c r="I27" s="1">
-        <v>1.5951457199871601E-2</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="J27" s="1">
-        <v>1.8800000000000001E-2</v>
+        <v>7.9000000000000008E-3</v>
       </c>
       <c r="K27" s="1">
-        <v>7.9000000000000008E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.4161000000000009E-3</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="0"/>
-        <v>4.4161000000000009E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.8348000000000002E-3</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="1"/>
-        <v>4.8348000000000002E-3</v>
-      </c>
-      <c r="N27" s="1">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="O27" s="1">
-        <f t="shared" si="2"/>
+      <c r="N27" s="2">
         <v>0.782418975653702</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:14">
       <c r="A28">
         <v>6</v>
       </c>
@@ -1793,31 +1687,27 @@
         <v>2.8899999999999999E-2</v>
       </c>
       <c r="I28" s="1">
-        <v>1.1346414637400999E-2</v>
+        <v>1.37E-2</v>
       </c>
       <c r="J28" s="1">
-        <v>1.37E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="K28" s="1">
-        <v>5.7999999999999996E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.2422000000000002E-3</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="0"/>
-        <v>3.2422000000000002E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.5495999999999995E-3</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="1"/>
-        <v>3.5495999999999995E-3</v>
-      </c>
-      <c r="N28" s="1">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="O28" s="1">
-        <f t="shared" si="2"/>
+      <c r="N28" s="2">
         <v>0.55654163796451894</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:14">
       <c r="A29">
         <v>6</v>
       </c>
@@ -1843,31 +1733,27 @@
         <v>1.41E-2</v>
       </c>
       <c r="I29" s="1">
-        <v>5.6837318515048398E-3</v>
+        <v>7.7999999999999996E-3</v>
       </c>
       <c r="J29" s="1">
-        <v>7.7999999999999996E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="K29" s="1">
-        <v>3.5999999999999999E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.0124000000000001E-3</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="0"/>
-        <v>2.0124000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.2031999999999998E-3</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="1"/>
-        <v>2.2031999999999998E-3</v>
-      </c>
-      <c r="N29" s="1">
         <v>7.6E-3</v>
       </c>
-      <c r="O29" s="1">
-        <f t="shared" si="2"/>
+      <c r="N29" s="2">
         <v>0.27878704731631243</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:14">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1893,31 +1779,27 @@
         <v>3.0999999999999999E-3</v>
       </c>
       <c r="I30" s="1">
-        <v>1.34562051271607E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="J30" s="1">
-        <v>2.5000000000000001E-3</v>
+        <v>1.4E-3</v>
       </c>
       <c r="K30" s="1">
+        <f t="shared" si="0"/>
+        <v>7.8260000000000005E-4</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="1"/>
+        <v>8.5680000000000001E-4</v>
+      </c>
+      <c r="M30" s="1">
         <v>1.4E-3</v>
       </c>
-      <c r="L30" s="1">
-        <f t="shared" si="0"/>
-        <v>7.8260000000000005E-4</v>
-      </c>
-      <c r="M30" s="1">
-        <f t="shared" si="1"/>
-        <v>8.5680000000000001E-4</v>
-      </c>
-      <c r="N30" s="1">
-        <v>1.4E-3</v>
-      </c>
-      <c r="O30" s="1">
-        <f t="shared" si="2"/>
+      <c r="N30" s="2">
         <v>6.6002686148723233E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:14">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1943,31 +1825,27 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="I31" s="1">
-        <v>1.9242498137626699E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="J31" s="1">
-        <v>5.9999999999999995E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="K31" s="1">
-        <v>4.0000000000000002E-4</v>
+        <f t="shared" si="0"/>
+        <v>2.2360000000000004E-4</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2360000000000004E-4</v>
+        <f t="shared" si="1"/>
+        <v>2.4479999999999999E-4</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="1"/>
-        <v>2.4479999999999999E-4</v>
-      </c>
-      <c r="N31" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="O31" s="1">
-        <f t="shared" si="2"/>
+      <c r="N31" s="2">
         <v>9.4384453365058962E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:14">
       <c r="A32">
         <v>6.5</v>
       </c>
@@ -1993,31 +1871,27 @@
         <v>0.53580000000000005</v>
       </c>
       <c r="I32" s="1">
-        <v>0.217410352404725</v>
+        <v>0.26340000000000002</v>
       </c>
       <c r="J32" s="1">
-        <v>0.26340000000000002</v>
+        <v>0.13239999999999999</v>
       </c>
       <c r="K32" s="1">
-        <v>0.13239999999999999</v>
+        <f t="shared" si="0"/>
+        <v>7.4011599999999997E-2</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="0"/>
-        <v>7.4011599999999997E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.1028799999999998E-2</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="1"/>
-        <v>8.1028799999999998E-2</v>
-      </c>
-      <c r="N32" s="1">
         <v>0.52339999999999998</v>
       </c>
-      <c r="O32" s="1">
-        <f t="shared" si="2"/>
+      <c r="N32" s="2">
         <v>10.663977785451761</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:14">
       <c r="A33">
         <v>6.5</v>
       </c>
@@ -2043,31 +1917,27 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="I33" s="1">
-        <v>0.167140135611346</v>
+        <v>0.20230000000000001</v>
       </c>
       <c r="J33" s="1">
-        <v>0.20230000000000001</v>
+        <v>0.1018</v>
       </c>
       <c r="K33" s="1">
-        <v>0.1018</v>
+        <f t="shared" si="0"/>
+        <v>5.6906200000000004E-2</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="0"/>
-        <v>5.6906200000000004E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.2301599999999999E-2</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="1"/>
-        <v>6.2301599999999999E-2</v>
-      </c>
-      <c r="N33" s="1">
         <v>0.40810000000000002</v>
       </c>
-      <c r="O33" s="1">
-        <f t="shared" si="2"/>
+      <c r="N33" s="2">
         <v>8.1982236517365212</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:14">
       <c r="A34">
         <v>6.5</v>
       </c>
@@ -2093,31 +1963,27 @@
         <v>0.2535</v>
       </c>
       <c r="I34" s="1">
-        <v>0.103062477565858</v>
+        <v>0.126</v>
       </c>
       <c r="J34" s="1">
-        <v>0.126</v>
+        <v>6.3299999999999995E-2</v>
       </c>
       <c r="K34" s="1">
-        <v>6.3299999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5384699999999998E-2</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="0"/>
-        <v>3.5384699999999998E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.8739599999999999E-2</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8739599999999999E-2</v>
-      </c>
-      <c r="N34" s="1">
         <v>0.2384</v>
       </c>
-      <c r="O34" s="1">
-        <f t="shared" si="2"/>
+      <c r="N34" s="2">
         <v>5.0552145246053346</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:14">
       <c r="A35">
         <v>6.5</v>
       </c>
@@ -2143,31 +2009,27 @@
         <v>0.17630000000000001</v>
       </c>
       <c r="I35" s="1">
-        <v>7.1865294783914804E-2</v>
+        <v>8.9099999999999999E-2</v>
       </c>
       <c r="J35" s="1">
-        <v>8.9099999999999999E-2</v>
+        <v>4.48E-2</v>
       </c>
       <c r="K35" s="1">
-        <v>4.48E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.5043200000000002E-2</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="0"/>
-        <v>2.5043200000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.74176E-2</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="1"/>
-        <v>2.74176E-2</v>
-      </c>
-      <c r="N35" s="1">
         <v>0.15390000000000001</v>
       </c>
-      <c r="O35" s="1">
-        <f t="shared" si="2"/>
+      <c r="N35" s="2">
         <v>3.5249927091510207</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:14">
       <c r="A36">
         <v>6.5</v>
       </c>
@@ -2193,31 +2055,27 @@
         <v>0.10539999999999999</v>
       </c>
       <c r="I36" s="1">
-        <v>4.3184481316979301E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="J36" s="1">
-        <v>5.5E-2</v>
+        <v>2.7699999999999999E-2</v>
       </c>
       <c r="K36" s="1">
-        <v>2.7699999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.5484300000000001E-2</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5484300000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6952399999999999E-2</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6952399999999999E-2</v>
-      </c>
-      <c r="N36" s="1">
         <v>8.1699999999999995E-2</v>
       </c>
-      <c r="O36" s="1">
-        <f t="shared" si="2"/>
+      <c r="N36" s="2">
         <v>2.1181988085978345</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:14">
       <c r="A37">
         <v>6.5</v>
       </c>
@@ -2243,31 +2101,27 @@
         <v>6.7100000000000007E-2</v>
       </c>
       <c r="I37" s="1">
-        <v>2.7683034468208099E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="J37" s="1">
-        <v>3.6299999999999999E-2</v>
+        <v>1.84E-2</v>
       </c>
       <c r="K37" s="1">
-        <v>1.84E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0285600000000001E-2</v>
       </c>
       <c r="L37" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0285600000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.12608E-2</v>
       </c>
       <c r="M37" s="1">
-        <f t="shared" si="1"/>
-        <v>1.12608E-2</v>
-      </c>
-      <c r="N37" s="1">
         <v>4.7199999999999999E-2</v>
       </c>
-      <c r="O37" s="1">
-        <f t="shared" si="2"/>
+      <c r="N37" s="2">
         <v>1.3578528406656072</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:14">
       <c r="A38">
         <v>6.5</v>
       </c>
@@ -2293,31 +2147,27 @@
         <v>4.7500000000000001E-2</v>
       </c>
       <c r="I38" s="1">
-        <v>1.9709648711849999E-2</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="J38" s="1">
-        <v>2.6599999999999999E-2</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="K38" s="1">
-        <v>1.3599999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.6024000000000005E-3</v>
       </c>
       <c r="L38" s="1">
-        <f t="shared" si="0"/>
-        <v>7.6024000000000005E-3</v>
+        <f t="shared" si="1"/>
+        <v>8.3231999999999993E-3</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="1"/>
-        <v>8.3231999999999993E-3</v>
-      </c>
-      <c r="N38" s="1">
         <v>3.1300000000000001E-2</v>
       </c>
-      <c r="O38" s="1">
-        <f t="shared" si="2"/>
+      <c r="N38" s="2">
         <v>0.96675826931624242</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:14">
       <c r="A39">
         <v>6.5</v>
       </c>
@@ -2343,31 +2193,27 @@
         <v>2.3199999999999998E-2</v>
       </c>
       <c r="I39" s="1">
-        <v>9.8775127788004093E-3</v>
+        <v>1.5100000000000001E-2</v>
       </c>
       <c r="J39" s="1">
-        <v>1.5100000000000001E-2</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="K39" s="1">
-        <v>8.3999999999999995E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.6956000000000003E-3</v>
       </c>
       <c r="L39" s="1">
-        <f t="shared" si="0"/>
-        <v>4.6956000000000003E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.1407999999999992E-3</v>
       </c>
       <c r="M39" s="1">
-        <f t="shared" si="1"/>
-        <v>5.1407999999999992E-3</v>
-      </c>
-      <c r="N39" s="1">
         <v>1.14E-2</v>
       </c>
-      <c r="O39" s="1">
-        <f t="shared" si="2"/>
+      <c r="N39" s="2">
         <v>0.48449200180016011</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:14">
       <c r="A40">
         <v>6.5</v>
       </c>
@@ -2393,31 +2239,27 @@
         <v>5.1999999999999998E-3</v>
       </c>
       <c r="I40" s="1">
-        <v>2.3388825976253299E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="J40" s="1">
-        <v>4.7999999999999996E-3</v>
+        <v>3.3E-3</v>
       </c>
       <c r="K40" s="1">
-        <v>3.3E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.8447000000000001E-3</v>
       </c>
       <c r="L40" s="1">
-        <f t="shared" si="0"/>
-        <v>1.8447000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.0195999999999999E-3</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0195999999999999E-3</v>
-      </c>
-      <c r="N40" s="1">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="O40" s="1">
-        <f t="shared" si="2"/>
+      <c r="N40" s="2">
         <v>0.11472219141352243</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:14">
       <c r="A41">
         <v>6.5</v>
       </c>
@@ -2443,31 +2285,27 @@
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="I41" s="1">
-        <v>3.3447503040091002E-4</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="J41" s="1">
-        <v>1.1000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="K41" s="1">
-        <v>1E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.5900000000000004E-4</v>
       </c>
       <c r="L41" s="1">
-        <f t="shared" si="0"/>
-        <v>5.5900000000000004E-4</v>
+        <f t="shared" si="1"/>
+        <v>6.1200000000000002E-4</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="1"/>
-        <v>6.1200000000000002E-4</v>
-      </c>
-      <c r="N41" s="1">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="O41" s="1">
-        <f t="shared" si="2"/>
+      <c r="N41" s="2">
         <v>1.6406000241164637E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:14">
       <c r="A42">
         <v>7</v>
       </c>
@@ -2493,31 +2331,27 @@
         <v>0.77149999999999996</v>
       </c>
       <c r="I42" s="1">
-        <v>0.34525917768541098</v>
+        <v>0.42559999999999998</v>
       </c>
       <c r="J42" s="1">
-        <v>0.42559999999999998</v>
+        <v>0.24510000000000001</v>
       </c>
       <c r="K42" s="1">
-        <v>0.24510000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.13701090000000002</v>
       </c>
       <c r="L42" s="1">
-        <f t="shared" si="0"/>
-        <v>0.13701090000000002</v>
+        <f t="shared" si="1"/>
+        <v>0.1500012</v>
       </c>
       <c r="M42" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1500012</v>
-      </c>
-      <c r="N42" s="1">
         <v>0.6915</v>
       </c>
-      <c r="O42" s="1">
-        <f t="shared" si="2"/>
+      <c r="N42" s="2">
         <v>16.934962665469406</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:14">
       <c r="A43">
         <v>7</v>
       </c>
@@ -2543,31 +2377,27 @@
         <v>0.61339999999999995</v>
       </c>
       <c r="I43" s="1">
-        <v>0.27441662770601399</v>
+        <v>0.3377</v>
       </c>
       <c r="J43" s="1">
-        <v>0.3377</v>
+        <v>0.19470000000000001</v>
       </c>
       <c r="K43" s="1">
-        <v>0.19470000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.10883730000000001</v>
       </c>
       <c r="L43" s="1">
-        <f t="shared" si="0"/>
-        <v>0.10883730000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.11915640000000001</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="1"/>
-        <v>0.11915640000000001</v>
-      </c>
-      <c r="N43" s="1">
         <v>0.55969999999999998</v>
       </c>
-      <c r="O43" s="1">
-        <f t="shared" si="2"/>
+      <c r="N43" s="2">
         <v>13.460135588979986</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:14">
       <c r="A44">
         <v>7</v>
       </c>
@@ -2593,31 +2423,27 @@
         <v>0.38950000000000001</v>
       </c>
       <c r="I44" s="1">
-        <v>0.17453637933327601</v>
+        <v>0.2167</v>
       </c>
       <c r="J44" s="1">
-        <v>0.2167</v>
+        <v>0.12479999999999999</v>
       </c>
       <c r="K44" s="1">
-        <v>0.12479999999999999</v>
+        <f t="shared" si="0"/>
+        <v>6.9763199999999997E-2</v>
       </c>
       <c r="L44" s="1">
-        <f t="shared" si="0"/>
-        <v>6.9763199999999997E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.637759999999999E-2</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="1"/>
-        <v>7.637759999999999E-2</v>
-      </c>
-      <c r="N44" s="1">
         <v>0.34300000000000003</v>
       </c>
-      <c r="O44" s="1">
-        <f t="shared" si="2"/>
+      <c r="N44" s="2">
         <v>8.5610094062971882</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:14">
       <c r="A45">
         <v>7</v>
       </c>
@@ -2643,31 +2469,27 @@
         <v>0.27360000000000001</v>
       </c>
       <c r="I45" s="1">
-        <v>0.12292199497176</v>
+        <v>0.15459999999999999</v>
       </c>
       <c r="J45" s="1">
-        <v>0.15459999999999999</v>
+        <v>8.9099999999999999E-2</v>
       </c>
       <c r="K45" s="1">
-        <v>8.9099999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9806900000000001E-2</v>
       </c>
       <c r="L45" s="1">
-        <f t="shared" si="0"/>
-        <v>4.9806900000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.45292E-2</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="1"/>
-        <v>5.45292E-2</v>
-      </c>
-      <c r="N45" s="1">
         <v>0.2258</v>
       </c>
-      <c r="O45" s="1">
-        <f t="shared" si="2"/>
+      <c r="N45" s="2">
         <v>6.0293238533648275</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:14">
       <c r="A46">
         <v>7</v>
       </c>
@@ -2693,31 +2515,27 @@
         <v>0.1646</v>
       </c>
       <c r="I46" s="1">
-        <v>7.4319328744490695E-2</v>
+        <v>9.5899999999999999E-2</v>
       </c>
       <c r="J46" s="1">
-        <v>9.5899999999999999E-2</v>
+        <v>5.5399999999999998E-2</v>
       </c>
       <c r="K46" s="1">
-        <v>5.5399999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.0968600000000002E-2</v>
       </c>
       <c r="L46" s="1">
-        <f t="shared" si="0"/>
-        <v>3.0968600000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.3904799999999999E-2</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" si="1"/>
-        <v>3.3904799999999999E-2</v>
-      </c>
-      <c r="N46" s="1">
         <v>0.12139999999999999</v>
       </c>
-      <c r="O46" s="1">
-        <f t="shared" si="2"/>
+      <c r="N46" s="2">
         <v>3.645363074917269</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:14">
       <c r="A47">
         <v>7</v>
       </c>
@@ -2743,31 +2561,27 @@
         <v>0.1051</v>
       </c>
       <c r="I47" s="1">
-        <v>4.77439974185358E-2</v>
+        <v>6.3500000000000001E-2</v>
       </c>
       <c r="J47" s="1">
-        <v>6.3500000000000001E-2</v>
+        <v>3.6900000000000002E-2</v>
       </c>
       <c r="K47" s="1">
-        <v>3.6900000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.0627100000000002E-2</v>
       </c>
       <c r="L47" s="1">
-        <f t="shared" si="0"/>
-        <v>2.0627100000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.25828E-2</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="1"/>
-        <v>2.25828E-2</v>
-      </c>
-      <c r="N47" s="1">
         <v>7.0499999999999993E-2</v>
       </c>
-      <c r="O47" s="1">
-        <f t="shared" si="2"/>
+      <c r="N47" s="2">
         <v>2.3418430733791809</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:14">
       <c r="A48">
         <v>7</v>
       </c>
@@ -2793,31 +2607,27 @@
         <v>7.4499999999999997E-2</v>
       </c>
       <c r="I48" s="1">
-        <v>3.4032403783347799E-2</v>
+        <v>4.65E-2</v>
       </c>
       <c r="J48" s="1">
-        <v>4.65E-2</v>
+        <v>2.7300000000000001E-2</v>
       </c>
       <c r="K48" s="1">
-        <v>2.7300000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.5260700000000002E-2</v>
       </c>
       <c r="L48" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5260700000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.67076E-2</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="1"/>
-        <v>1.67076E-2</v>
-      </c>
-      <c r="N48" s="1">
         <v>4.6899999999999997E-2</v>
       </c>
-      <c r="O48" s="1">
-        <f t="shared" si="2"/>
+      <c r="N48" s="2">
         <v>1.6692894055732097</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:14">
       <c r="A49">
         <v>7</v>
       </c>
@@ -2843,31 +2653,27 @@
         <v>3.6400000000000002E-2</v>
       </c>
       <c r="I49" s="1">
-        <v>1.7064910543578601E-2</v>
+        <v>2.64E-2</v>
       </c>
       <c r="J49" s="1">
-        <v>2.64E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="K49" s="1">
-        <v>1.6799999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.3912000000000006E-3</v>
       </c>
       <c r="L49" s="1">
-        <f t="shared" si="0"/>
-        <v>9.3912000000000006E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.0281599999999998E-2</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0281599999999998E-2</v>
-      </c>
-      <c r="N49" s="1">
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="O49" s="1">
-        <f t="shared" si="2"/>
+      <c r="N49" s="2">
         <v>0.8370338621625304</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:14">
       <c r="A50">
         <v>7</v>
       </c>
@@ -2893,31 +2699,27 @@
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="I50" s="1">
-        <v>4.0416146236942002E-3</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="J50" s="1">
-        <v>8.5000000000000006E-3</v>
+        <v>6.6E-3</v>
       </c>
       <c r="K50" s="1">
-        <v>6.6E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.6894000000000002E-3</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" si="0"/>
-        <v>3.6894000000000002E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.0391999999999997E-3</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="1"/>
-        <v>4.0391999999999997E-3</v>
-      </c>
-      <c r="N50" s="1">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="O50" s="1">
-        <f t="shared" si="2"/>
+      <c r="N50" s="2">
         <v>0.19824119729220052</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:14">
       <c r="A51">
         <v>7</v>
       </c>
@@ -2943,31 +2745,27 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="I51" s="1">
-        <v>5.7800392664122404E-4</v>
+        <v>1.9E-3</v>
       </c>
       <c r="J51" s="1">
-        <v>1.9E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="K51" s="1">
-        <v>2.0999999999999999E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.1739000000000001E-3</v>
       </c>
       <c r="L51" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1739000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.2851999999999998E-3</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2851999999999998E-3</v>
-      </c>
-      <c r="N51" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O51" s="1">
-        <f t="shared" si="2"/>
+      <c r="N51" s="2">
         <v>2.8351092601752038E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:14">
       <c r="A52">
         <v>7.5</v>
       </c>
@@ -2993,31 +2791,27 @@
         <v>1.0522</v>
       </c>
       <c r="I52" s="1">
-        <v>0.54276873883284404</v>
+        <v>0.61960000000000004</v>
       </c>
       <c r="J52" s="1">
-        <v>0.61960000000000004</v>
+        <v>0.38690000000000002</v>
       </c>
       <c r="K52" s="1">
-        <v>0.38690000000000002</v>
+        <f t="shared" si="0"/>
+        <v>0.21627710000000003</v>
       </c>
       <c r="L52" s="1">
-        <f t="shared" si="0"/>
-        <v>0.21627710000000003</v>
+        <f t="shared" si="1"/>
+        <v>0.23678280000000002</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" si="1"/>
-        <v>0.23678280000000002</v>
-      </c>
-      <c r="N52" s="1">
         <v>0.90990000000000004</v>
       </c>
-      <c r="O52" s="1">
-        <f t="shared" si="2"/>
+      <c r="N52" s="2">
         <v>26.622806639751001</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:14">
       <c r="A53">
         <v>7.5</v>
       </c>
@@ -3043,31 +2837,27 @@
         <v>0.86319999999999997</v>
       </c>
       <c r="I53" s="1">
-        <v>0.44508486999264302</v>
+        <v>0.5071</v>
       </c>
       <c r="J53" s="1">
-        <v>0.5071</v>
+        <v>0.317</v>
       </c>
       <c r="K53" s="1">
-        <v>0.317</v>
+        <f t="shared" si="0"/>
+        <v>0.17720300000000003</v>
       </c>
       <c r="L53" s="1">
-        <f t="shared" si="0"/>
-        <v>0.17720300000000003</v>
+        <f t="shared" si="1"/>
+        <v>0.19400400000000001</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" si="1"/>
-        <v>0.19400400000000001</v>
-      </c>
-      <c r="N53" s="1">
         <v>0.76139999999999997</v>
       </c>
-      <c r="O53" s="1">
-        <f t="shared" si="2"/>
+      <c r="N53" s="2">
         <v>21.83141287313914</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:14">
       <c r="A54">
         <v>7.5</v>
       </c>
@@ -3093,31 +2883,27 @@
         <v>0.56679999999999997</v>
       </c>
       <c r="I54" s="1">
-        <v>0.292661174709067</v>
+        <v>0.3357</v>
       </c>
       <c r="J54" s="1">
-        <v>0.3357</v>
+        <v>0.2099</v>
       </c>
       <c r="K54" s="1">
-        <v>0.2099</v>
+        <f t="shared" si="0"/>
+        <v>0.11733410000000001</v>
       </c>
       <c r="L54" s="1">
-        <f t="shared" si="0"/>
-        <v>0.11733410000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.12845880000000001</v>
       </c>
       <c r="M54" s="1">
-        <f t="shared" si="1"/>
-        <v>0.12845880000000001</v>
-      </c>
-      <c r="N54" s="1">
         <v>0.4899</v>
       </c>
-      <c r="O54" s="1">
-        <f t="shared" si="2"/>
+      <c r="N54" s="2">
         <v>14.355030619479738</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:14">
       <c r="A55">
         <v>7.5</v>
       </c>
@@ -3143,31 +2929,27 @@
         <v>0.40289999999999998</v>
       </c>
       <c r="I55" s="1">
-        <v>0.208538758787775</v>
+        <v>0.2422</v>
       </c>
       <c r="J55" s="1">
-        <v>0.2422</v>
+        <v>0.1515</v>
       </c>
       <c r="K55" s="1">
-        <v>0.1515</v>
+        <f t="shared" si="0"/>
+        <v>8.46885E-2</v>
       </c>
       <c r="L55" s="1">
-        <f t="shared" si="0"/>
-        <v>8.46885E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.2717999999999995E-2</v>
       </c>
       <c r="M55" s="1">
-        <f t="shared" si="1"/>
-        <v>9.2717999999999995E-2</v>
-      </c>
-      <c r="N55" s="1">
         <v>0.3296</v>
       </c>
-      <c r="O55" s="1">
-        <f t="shared" si="2"/>
+      <c r="N55" s="2">
         <v>10.228826118540365</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:14">
       <c r="A56">
         <v>7.5</v>
       </c>
@@ -3193,31 +2975,27 @@
         <v>0.2442</v>
       </c>
       <c r="I56" s="1">
-        <v>0.12702845334854301</v>
+        <v>0.15129999999999999</v>
       </c>
       <c r="J56" s="1">
-        <v>0.15129999999999999</v>
+        <v>9.4899999999999998E-2</v>
       </c>
       <c r="K56" s="1">
-        <v>9.4899999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.3049100000000002E-2</v>
       </c>
       <c r="L56" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3049100000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.80788E-2</v>
       </c>
       <c r="M56" s="1">
-        <f t="shared" si="1"/>
-        <v>5.80788E-2</v>
-      </c>
-      <c r="N56" s="1">
         <v>0.18</v>
       </c>
-      <c r="O56" s="1">
-        <f t="shared" si="2"/>
+      <c r="N56" s="2">
         <v>6.2307456367460343</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:14">
       <c r="A57">
         <v>7.5</v>
       </c>
@@ -3243,31 +3021,27 @@
         <v>0.15629999999999999</v>
       </c>
       <c r="I57" s="1">
-        <v>8.18223751009612E-2</v>
+        <v>0.1004</v>
       </c>
       <c r="J57" s="1">
-        <v>0.1004</v>
+        <v>6.3399999999999998E-2</v>
       </c>
       <c r="K57" s="1">
-        <v>6.3399999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5440600000000003E-2</v>
       </c>
       <c r="L57" s="1">
-        <f t="shared" si="0"/>
-        <v>3.5440600000000003E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.8800799999999996E-2</v>
       </c>
       <c r="M57" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8800799999999996E-2</v>
-      </c>
-      <c r="N57" s="1">
         <v>0.1052</v>
       </c>
-      <c r="O57" s="1">
-        <f t="shared" si="2"/>
+      <c r="N57" s="2">
         <v>4.0133874987021469</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:14">
       <c r="A58">
         <v>7.5</v>
       </c>
@@ -3293,31 +3067,27 @@
         <v>0.111</v>
       </c>
       <c r="I58" s="1">
-        <v>5.8409189549371299E-2</v>
+        <v>7.3599999999999999E-2</v>
       </c>
       <c r="J58" s="1">
-        <v>7.3599999999999999E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="K58" s="1">
-        <v>4.7E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.6273000000000001E-2</v>
       </c>
       <c r="L58" s="1">
-        <f t="shared" si="0"/>
-        <v>2.6273000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.8763999999999998E-2</v>
       </c>
       <c r="M58" s="1">
-        <f t="shared" si="1"/>
-        <v>2.8763999999999998E-2</v>
-      </c>
-      <c r="N58" s="1">
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="O58" s="1">
-        <f t="shared" si="2"/>
+      <c r="N58" s="2">
         <v>2.8649707473966624</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:14">
       <c r="A59">
         <v>7.5</v>
       </c>
@@ -3343,31 +3113,27 @@
         <v>5.4300000000000001E-2</v>
       </c>
       <c r="I59" s="1">
-        <v>2.93086834829526E-2</v>
+        <v>4.1799999999999997E-2</v>
       </c>
       <c r="J59" s="1">
-        <v>4.1799999999999997E-2</v>
+        <v>2.8899999999999999E-2</v>
       </c>
       <c r="K59" s="1">
-        <v>2.8899999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.6155100000000002E-2</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6155100000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.7686799999999999E-2</v>
       </c>
       <c r="M59" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7686799999999999E-2</v>
-      </c>
-      <c r="N59" s="1">
         <v>2.5700000000000001E-2</v>
       </c>
-      <c r="O59" s="1">
-        <f t="shared" si="2"/>
+      <c r="N59" s="2">
         <v>1.437590924838825</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:14">
       <c r="A60">
         <v>7.5</v>
       </c>
@@ -3393,31 +3159,27 @@
         <v>1.21E-2</v>
       </c>
       <c r="I60" s="1">
-        <v>6.9432075084186603E-3</v>
+        <v>1.34E-2</v>
       </c>
       <c r="J60" s="1">
-        <v>1.34E-2</v>
+        <v>1.14E-2</v>
       </c>
       <c r="K60" s="1">
-        <v>1.14E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.3726000000000008E-3</v>
       </c>
       <c r="L60" s="1">
-        <f t="shared" si="0"/>
-        <v>6.3726000000000008E-3</v>
+        <f t="shared" si="1"/>
+        <v>6.9768E-3</v>
       </c>
       <c r="M60" s="1">
-        <f t="shared" si="1"/>
-        <v>6.9768E-3</v>
-      </c>
-      <c r="N60" s="1">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="O60" s="1">
-        <f t="shared" si="2"/>
+      <c r="N60" s="2">
         <v>0.34056432828793526</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:14">
       <c r="A61">
         <v>7.5</v>
       </c>
@@ -3443,31 +3205,27 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="I61" s="1">
-        <v>9.9302890982502908E-4</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="J61" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="K61" s="1">
-        <v>3.5000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.9565000000000003E-3</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9565000000000003E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.1419999999999998E-3</v>
       </c>
       <c r="M61" s="1">
-        <f t="shared" si="1"/>
-        <v>2.1419999999999998E-3</v>
-      </c>
-      <c r="N61" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="O61" s="1">
-        <f t="shared" si="2"/>
+      <c r="N61" s="2">
         <v>4.8708068026917677E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:14">
       <c r="A62">
         <v>8</v>
       </c>
@@ -3493,31 +3251,27 @@
         <v>1.3597999999999999</v>
       </c>
       <c r="I62" s="1">
-        <v>0.84506551135814001</v>
+        <v>0.81320000000000003</v>
       </c>
       <c r="J62" s="1">
-        <v>0.81320000000000003</v>
+        <v>0.52100000000000002</v>
       </c>
       <c r="K62" s="1">
-        <v>0.52100000000000002</v>
+        <f t="shared" si="0"/>
+        <v>0.29123900000000003</v>
       </c>
       <c r="L62" s="1">
-        <f t="shared" si="0"/>
-        <v>0.29123900000000003</v>
+        <f t="shared" si="1"/>
+        <v>0.31885200000000002</v>
       </c>
       <c r="M62" s="1">
-        <f t="shared" si="1"/>
-        <v>0.31885200000000002</v>
-      </c>
-      <c r="N62" s="1">
         <v>1.1931</v>
       </c>
-      <c r="O62" s="1">
-        <f t="shared" si="2"/>
+      <c r="N62" s="2">
         <v>41.450463332116769</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:14">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3543,31 +3297,27 @@
         <v>1.1479999999999999</v>
       </c>
       <c r="I63" s="1">
-        <v>0.71314748379118698</v>
+        <v>0.68479999999999996</v>
       </c>
       <c r="J63" s="1">
-        <v>0.68479999999999996</v>
+        <v>0.43940000000000001</v>
       </c>
       <c r="K63" s="1">
-        <v>0.43940000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.24562460000000003</v>
       </c>
       <c r="L63" s="1">
-        <f t="shared" si="0"/>
-        <v>0.24562460000000003</v>
+        <f t="shared" si="1"/>
+        <v>0.26891280000000001</v>
       </c>
       <c r="M63" s="1">
-        <f t="shared" si="1"/>
-        <v>0.26891280000000001</v>
-      </c>
-      <c r="N63" s="1">
         <v>1.028</v>
       </c>
-      <c r="O63" s="1">
-        <f t="shared" si="2"/>
+      <c r="N63" s="2">
         <v>34.979884079957721</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:14">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3593,31 +3343,27 @@
         <v>0.78090000000000004</v>
       </c>
       <c r="I64" s="1">
-        <v>0.48560816264034901</v>
+        <v>0.46879999999999999</v>
       </c>
       <c r="J64" s="1">
-        <v>0.46879999999999999</v>
+        <v>0.30109999999999998</v>
       </c>
       <c r="K64" s="1">
-        <v>0.30109999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.16831490000000002</v>
       </c>
       <c r="L64" s="1">
-        <f t="shared" si="0"/>
-        <v>0.16831490000000002</v>
+        <f t="shared" si="1"/>
+        <v>0.18427319999999997</v>
       </c>
       <c r="M64" s="1">
-        <f t="shared" si="1"/>
-        <v>0.18427319999999997</v>
-      </c>
-      <c r="N64" s="1">
         <v>0.69440000000000002</v>
       </c>
-      <c r="O64" s="1">
-        <f t="shared" si="2"/>
+      <c r="N64" s="2">
         <v>23.819080377509117</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:14">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3643,31 +3389,27 @@
         <v>0.56279999999999997</v>
       </c>
       <c r="I65" s="1">
-        <v>0.350743477211167</v>
+        <v>0.34239999999999998</v>
       </c>
       <c r="J65" s="1">
-        <v>0.34239999999999998</v>
+        <v>0.22</v>
       </c>
       <c r="K65" s="1">
-        <v>0.22</v>
+        <f t="shared" si="0"/>
+        <v>0.12298000000000001</v>
       </c>
       <c r="L65" s="1">
-        <f t="shared" si="0"/>
-        <v>0.12298000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.13464000000000001</v>
       </c>
       <c r="M65" s="1">
-        <f t="shared" si="1"/>
-        <v>0.13464000000000001</v>
-      </c>
-      <c r="N65" s="1">
         <v>0.47860000000000003</v>
       </c>
-      <c r="O65" s="1">
-        <f t="shared" si="2"/>
+      <c r="N65" s="2">
         <v>17.20396755720774</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:14">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3693,31 +3435,27 @@
         <v>0.34420000000000001</v>
       </c>
       <c r="I66" s="1">
-        <v>0.21558690583137</v>
+        <v>0.21560000000000001</v>
       </c>
       <c r="J66" s="1">
-        <v>0.21560000000000001</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="K66" s="1">
-        <v>0.13900000000000001</v>
+        <f t="shared" si="0"/>
+        <v>7.770100000000002E-2</v>
       </c>
       <c r="L66" s="1">
-        <f t="shared" si="0"/>
-        <v>7.770100000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.5068000000000005E-2</v>
       </c>
       <c r="M66" s="1">
-        <f t="shared" si="1"/>
-        <v>8.5068000000000005E-2</v>
-      </c>
-      <c r="N66" s="1">
         <v>0.26619999999999999</v>
       </c>
-      <c r="O66" s="1">
-        <f t="shared" si="2"/>
+      <c r="N66" s="2">
         <v>10.574537731028698</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:14">
       <c r="A67">
         <v>8</v>
       </c>
@@ -3743,31 +3481,27 @@
         <v>0.22109999999999999</v>
       </c>
       <c r="I67" s="1">
-        <v>0.13932201667142999</v>
+        <v>0.14349999999999999</v>
       </c>
       <c r="J67" s="1">
-        <v>0.14349999999999999</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="K67" s="1">
-        <v>9.3200000000000005E-2</v>
+        <f t="shared" ref="K67:K71" si="2">J67*0.559</f>
+        <v>5.2098800000000008E-2</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" ref="L67:L71" si="3">K67*0.559</f>
-        <v>5.2098800000000008E-2</v>
+        <f t="shared" ref="L67:L71" si="3">J67*0.612</f>
+        <v>5.7038400000000003E-2</v>
       </c>
       <c r="M67" s="1">
-        <f t="shared" ref="M67:M71" si="4">K67*0.612</f>
-        <v>5.7038400000000003E-2</v>
-      </c>
-      <c r="N67" s="1">
         <v>0.15659999999999999</v>
       </c>
-      <c r="O67" s="1">
-        <f t="shared" ref="O67:O71" si="5">I67*981/20</f>
+      <c r="N67" s="2">
         <v>6.8337449177336413</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:14">
       <c r="A68">
         <v>8</v>
       </c>
@@ -3793,31 +3527,27 @@
         <v>0.1573</v>
       </c>
       <c r="I68" s="1">
-        <v>9.96371421329353E-2</v>
+        <v>0.10539999999999999</v>
       </c>
       <c r="J68" s="1">
-        <v>0.10539999999999999</v>
+        <v>6.9199999999999998E-2</v>
       </c>
       <c r="K68" s="1">
-        <v>6.9199999999999998E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.8682800000000003E-2</v>
       </c>
       <c r="L68" s="1">
         <f t="shared" si="3"/>
-        <v>3.8682800000000003E-2</v>
+        <v>4.2350399999999996E-2</v>
       </c>
       <c r="M68" s="1">
-        <f t="shared" si="4"/>
-        <v>4.2350399999999996E-2</v>
-      </c>
-      <c r="N68" s="1">
         <v>0.1047</v>
       </c>
-      <c r="O68" s="1">
-        <f t="shared" si="5"/>
+      <c r="N68" s="2">
         <v>4.8872018216204767</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:14">
       <c r="A69">
         <v>8</v>
       </c>
@@ -3843,31 +3573,27 @@
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="I69" s="1">
-        <v>5.0039887014293502E-2</v>
+        <v>5.9799999999999999E-2</v>
       </c>
       <c r="J69" s="1">
-        <v>5.9799999999999999E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="K69" s="1">
-        <v>4.2500000000000003E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.3757500000000004E-2</v>
       </c>
       <c r="L69" s="1">
         <f t="shared" si="3"/>
-        <v>2.3757500000000004E-2</v>
+        <v>2.6010000000000002E-2</v>
       </c>
       <c r="M69" s="1">
-        <f t="shared" si="4"/>
-        <v>2.6010000000000002E-2</v>
-      </c>
-      <c r="N69" s="1">
         <v>3.85E-2</v>
       </c>
-      <c r="O69" s="1">
-        <f t="shared" si="5"/>
+      <c r="N69" s="2">
         <v>2.4544564580510961</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:14">
       <c r="A70">
         <v>8</v>
       </c>
@@ -3893,31 +3619,27 @@
         <v>1.72E-2</v>
       </c>
       <c r="I70" s="1">
-        <v>1.18582824165172E-2</v>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="J70" s="1">
-        <v>1.9199999999999998E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="K70" s="1">
-        <v>1.6799999999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>9.3912000000000006E-3</v>
       </c>
       <c r="L70" s="1">
         <f t="shared" si="3"/>
-        <v>9.3912000000000006E-3</v>
+        <v>1.0281599999999998E-2</v>
       </c>
       <c r="M70" s="1">
-        <f t="shared" si="4"/>
-        <v>1.0281599999999998E-2</v>
-      </c>
-      <c r="N70" s="1">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="O70" s="1">
-        <f t="shared" si="5"/>
+      <c r="N70" s="2">
         <v>0.58164875253016868</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:14">
       <c r="A71">
         <v>8</v>
       </c>
@@ -3943,27 +3665,23 @@
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="I71" s="1">
-        <v>1.69611767946806E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="J71" s="1">
-        <v>4.3E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="K71" s="1">
-        <v>5.1999999999999998E-3</v>
+        <f t="shared" si="2"/>
+        <v>2.9068000000000002E-3</v>
       </c>
       <c r="L71" s="1">
         <f t="shared" si="3"/>
-        <v>2.9068000000000002E-3</v>
+        <v>3.1823999999999997E-3</v>
       </c>
       <c r="M71" s="1">
-        <f t="shared" si="4"/>
-        <v>3.1823999999999997E-3</v>
-      </c>
-      <c r="N71" s="1">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="O71" s="1">
-        <f t="shared" si="5"/>
+      <c r="N71" s="2">
         <v>8.3194572177908349E-2</v>
       </c>
     </row>

</xml_diff>